<commit_message>
Day by day / hour by hour relationships
</commit_message>
<xml_diff>
--- a/DOWdataset.xlsx
+++ b/DOWdataset.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FC32643-10D1-4FCD-9296-AA5E26EDF277}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A4C684-5DEA-4BEB-AB4F-28097326E833}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18168" windowHeight="8232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18165" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,12 +373,12 @@
   <dimension ref="A1:K169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,7 +448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -483,7 +483,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -518,7 +518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -588,7 +588,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -623,7 +623,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -658,7 +658,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -728,7 +728,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -798,7 +798,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -833,7 +833,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -868,7 +868,7 @@
         <v>4009</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -903,7 +903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -938,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -973,7 +973,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>5861</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>9387</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>4</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>6796</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>5</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>5</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>5</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>5</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>5</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>16755</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>5</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>5</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>5</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>5</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>2446</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>5</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>5</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>5</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>5</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>5</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>5</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>5</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>5</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>5</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>5</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>6</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>6</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>6</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>6</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>6</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>6</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>6</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>6</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>6</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>6</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>2905</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>6</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>6</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>6</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>6</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>6</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>6</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>6</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>6</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>6</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>6</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>6</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>6</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>6</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>7</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>7</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>7</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>7</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>7</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>7</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>7</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>7</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>7</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>7</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>7</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>7</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>7</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3317</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>7</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>7</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>7</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>7</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>7</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>7</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>7</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>7</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>7</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>7</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Created synthetic average week by applying poisson to dataframe
</commit_message>
<xml_diff>
--- a/DOWdataset.xlsx
+++ b/DOWdataset.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A4C684-5DEA-4BEB-AB4F-28097326E833}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7681E2A-A743-4852-BB64-C91ADBBE6493}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18165" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18168" windowHeight="8232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,12 +373,12 @@
   <dimension ref="A1:K169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="K158" sqref="K158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -448,7 +448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -483,7 +483,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -518,7 +518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -588,7 +588,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -623,7 +623,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -658,7 +658,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -693,7 +693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -728,7 +728,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -798,7 +798,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -833,7 +833,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -868,7 +868,7 @@
         <v>4009</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -903,7 +903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -938,7 +938,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -973,7 +973,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>2346</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>2243</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>5861</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>2159</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>3</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>3</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>2063</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>2297</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>9387</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>2649</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>4</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>2061</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>6796</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>2667</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>5</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>5</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>5</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>5</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>5</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>5</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>5</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>5</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>5</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>16755</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>5</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>5</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>5</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>6579</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>5</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>2446</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>5</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>2207</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>5</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>5</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>5</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>5</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>5</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>5</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>5</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>5</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>6</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>6</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>6</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>6</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>6</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>6</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>6</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>6</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>6</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>2270</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>6</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>2896</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>6</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>2905</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>6</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>2066</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>6</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>6</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>6</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>6</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>6</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>6</v>
       </c>
@@ -5278,7 +5278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>6</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>6</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>6</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>6</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>7</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>7</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>7</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>7</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>7</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>7</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>7</v>
       </c>
@@ -5698,7 +5698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>7</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>7</v>
       </c>
@@ -5768,7 +5768,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>7</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>7</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>7</v>
       </c>
@@ -5873,7 +5873,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>7</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3317</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>7</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>7</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>7</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>7</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>7</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>7</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>7</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>7</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>7</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>7</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>7</v>
       </c>

</xml_diff>